<commit_message>
Added functionality of the Diagnosis.java class. test results now are saved in the excel files + Added gender field to Patient.java. changed hashtable type to String Double + Added right to left slide transition animations in SlideTransitions.java
</commit_message>
<xml_diff>
--- a/PatientList.xlsx
+++ b/PatientList.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abada\IdeaProjects\Medical-Diagnosis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97252\Desktop\Medical-Diagnosis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2925F5FA-70FE-4A7C-9EF4-ECC8AEB18ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1AFE3C-3B4A-4E9B-9E3A-95D50A88BA47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33818" yWindow="68" windowWidth="16200" windowHeight="9847" xr2:uid="{D2BC487A-35A7-4E1F-8D4A-67F57BDA3325}"/>
+    <workbookView xWindow="-24684" yWindow="-108" windowWidth="24792" windowHeight="14856" xr2:uid="{D2BC487A-35A7-4E1F-8D4A-67F57BDA3325}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>firstname</t>
   </si>
@@ -46,25 +46,50 @@
     <t>asd</t>
   </si>
   <si>
-    <t>sdaf</t>
-  </si>
-  <si>
-    <t>dasf</t>
-  </si>
-  <si>
     <t>Blood Type</t>
   </si>
   <si>
     <t>dsf</t>
   </si>
   <si>
-    <t>ewr</t>
+    <t>fadi</t>
+  </si>
+  <si>
+    <t>badarni</t>
+  </si>
+  <si>
+    <t>O+</t>
+  </si>
+  <si>
+    <t>ahmad</t>
+  </si>
+  <si>
+    <t>sh</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>abed</t>
+  </si>
+  <si>
+    <t>ak</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Male</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -423,19 +448,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D788D7CC-192B-4F5D-85B5-B142119D78B6}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.77734375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.0"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>207527979</v>
       </c>
@@ -458,10 +484,13 @@
         <v>586535522</v>
       </c>
       <c r="H1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>12213</v>
       </c>
@@ -484,59 +513,97 @@
         <v>12431</v>
       </c>
       <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>209315647</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
+      <c r="D3">
+        <v>23</v>
+      </c>
+      <c r="E3">
+        <v>82</v>
+      </c>
+      <c r="F3">
+        <v>184</v>
+      </c>
+      <c r="G3">
+        <v>524183083</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>12213</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>123456789</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <v>80</v>
+      </c>
+      <c r="F4">
+        <v>180</v>
+      </c>
+      <c r="G4">
+        <v>15241830</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1.23435234E8</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="E3">
-        <v>34</v>
-      </c>
-      <c r="F3">
-        <v>324</v>
-      </c>
-      <c r="G3">
-        <v>324</v>
-      </c>
-      <c r="H3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>1324</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>231</v>
-      </c>
-      <c r="E4">
-        <v>324</v>
-      </c>
-      <c r="F4">
-        <v>324</v>
-      </c>
-      <c r="G4">
-        <v>34</v>
-      </c>
-      <c r="H4" t="s">
-        <v>7</v>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>79.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>176.0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>5.24111123E8</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>